<commit_message>
Added the HumanPlayer class, as it had not been added Added the tests for disproving suggestions
</commit_message>
<xml_diff>
--- a/Finalized Board Layout.xlsx
+++ b/Finalized Board Layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,12 +220,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -243,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -370,23 +364,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -432,8 +411,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -454,29 +435,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -499,6 +469,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -521,6 +492,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -852,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z26" sqref="B2:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -955,7 +927,7 @@
       <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="27" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1003,7 +975,7 @@
       <c r="U2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="V2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="W2" s="12" t="s">
@@ -1495,7 +1467,7 @@
       <c r="Y8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Z8" s="34" t="s">
+      <c r="Z8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="AB8" s="15" t="s">
@@ -2419,7 +2391,7 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -2494,7 +2466,7 @@
       <c r="Z20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE20" s="35"/>
+      <c r="AE20" s="24"/>
     </row>
     <row r="21" spans="1:33">
       <c r="A21">
@@ -2575,7 +2547,7 @@
       <c r="Z21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE21" s="35"/>
+      <c r="AE21" s="24"/>
     </row>
     <row r="22" spans="1:33">
       <c r="A22">
@@ -2656,7 +2628,7 @@
       <c r="Z22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE22" s="35"/>
+      <c r="AE22" s="24"/>
     </row>
     <row r="23" spans="1:33">
       <c r="A23">
@@ -2737,7 +2709,7 @@
       <c r="Z23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE23" s="35"/>
+      <c r="AE23" s="24"/>
     </row>
     <row r="24" spans="1:33">
       <c r="A24">
@@ -2818,7 +2790,7 @@
       <c r="Z24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE24" s="35"/>
+      <c r="AE24" s="24"/>
     </row>
     <row r="25" spans="1:33">
       <c r="A25">
@@ -2899,7 +2871,7 @@
       <c r="Z25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE25" s="35"/>
+      <c r="AE25" s="24"/>
     </row>
     <row r="26" spans="1:33">
       <c r="A26">
@@ -2932,7 +2904,7 @@
       <c r="J26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="40" t="s">
+      <c r="K26" s="29" t="s">
         <v>4</v>
       </c>
       <c r="L26" s="9" t="s">
@@ -2950,7 +2922,7 @@
       <c r="P26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Q26" s="39" t="s">
+      <c r="Q26" s="28" t="s">
         <v>4</v>
       </c>
       <c r="R26" s="4" t="s">
@@ -2980,84 +2952,84 @@
       <c r="Z26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AB26" s="32"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="32"/>
-      <c r="AE26" s="36"/>
-      <c r="AF26" s="32"/>
-      <c r="AG26" s="32"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
     </row>
     <row r="27" spans="1:33">
-      <c r="AB27" s="32"/>
-      <c r="AC27" s="32"/>
-      <c r="AD27" s="32"/>
-      <c r="AE27" s="36"/>
-      <c r="AF27" s="32"/>
-      <c r="AG27" s="32"/>
+      <c r="AB27" s="21"/>
+      <c r="AC27" s="21"/>
+      <c r="AD27" s="21"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="21"/>
+      <c r="AG27" s="21"/>
     </row>
     <row r="28" spans="1:33">
-      <c r="AB28" s="32"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="32"/>
-      <c r="AE28" s="36"/>
-      <c r="AF28" s="32"/>
-      <c r="AG28" s="32"/>
+      <c r="AB28" s="21"/>
+      <c r="AC28" s="21"/>
+      <c r="AD28" s="21"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="21"/>
+      <c r="AG28" s="21"/>
     </row>
     <row r="29" spans="1:33">
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="36"/>
-      <c r="AF29" s="32"/>
-      <c r="AG29" s="32"/>
+      <c r="AB29" s="21"/>
+      <c r="AC29" s="21"/>
+      <c r="AD29" s="21"/>
+      <c r="AE29" s="25"/>
+      <c r="AF29" s="21"/>
+      <c r="AG29" s="21"/>
     </row>
     <row r="30" spans="1:33">
-      <c r="AB30" s="32"/>
-      <c r="AC30" s="32"/>
-      <c r="AD30" s="32"/>
-      <c r="AE30" s="36"/>
-      <c r="AF30" s="32"/>
-      <c r="AG30" s="32"/>
+      <c r="AB30" s="21"/>
+      <c r="AC30" s="21"/>
+      <c r="AD30" s="21"/>
+      <c r="AE30" s="25"/>
+      <c r="AF30" s="21"/>
+      <c r="AG30" s="21"/>
     </row>
     <row r="31" spans="1:33">
-      <c r="AB31" s="32"/>
-      <c r="AC31" s="33"/>
-      <c r="AD31" s="32"/>
-      <c r="AE31" s="36"/>
-      <c r="AF31" s="32"/>
-      <c r="AG31" s="32"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="22"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="21"/>
     </row>
     <row r="32" spans="1:33">
-      <c r="AB32" s="32"/>
-      <c r="AC32" s="32"/>
-      <c r="AD32" s="32"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="32"/>
-      <c r="AG32" s="32"/>
+      <c r="AB32" s="21"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="25"/>
+      <c r="AF32" s="21"/>
+      <c r="AG32" s="21"/>
     </row>
     <row r="33" spans="28:33">
-      <c r="AB33" s="32"/>
-      <c r="AC33" s="32"/>
-      <c r="AD33" s="32"/>
-      <c r="AE33" s="36"/>
-      <c r="AF33" s="32"/>
-      <c r="AG33" s="32"/>
+      <c r="AB33" s="21"/>
+      <c r="AC33" s="21"/>
+      <c r="AD33" s="21"/>
+      <c r="AE33" s="25"/>
+      <c r="AF33" s="21"/>
+      <c r="AG33" s="21"/>
     </row>
     <row r="34" spans="28:33">
-      <c r="AB34" s="32"/>
-      <c r="AC34" s="32"/>
-      <c r="AD34" s="32"/>
-      <c r="AE34" s="36"/>
-      <c r="AF34" s="32"/>
-      <c r="AG34" s="32"/>
+      <c r="AB34" s="21"/>
+      <c r="AC34" s="21"/>
+      <c r="AD34" s="21"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="21"/>
+      <c r="AG34" s="21"/>
     </row>
     <row r="35" spans="28:33">
-      <c r="AB35" s="32"/>
-      <c r="AC35" s="32"/>
-      <c r="AD35" s="32"/>
-      <c r="AE35" s="32"/>
-      <c r="AF35" s="32"/>
-      <c r="AG35" s="32"/>
+      <c r="AB35" s="21"/>
+      <c r="AC35" s="21"/>
+      <c r="AD35" s="21"/>
+      <c r="AE35" s="21"/>
+      <c r="AF35" s="21"/>
+      <c r="AG35" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3074,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N42" sqref="C32:N42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3181,11 +3153,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F2" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G2" s="23">
+      <c r="F2" s="27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -3245,7 +3217,7 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="26">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -3266,7 +3238,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16" thickBot="1">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3371,7 +3343,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="16" thickBot="1">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3427,7 +3399,7 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="7">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
@@ -3476,7 +3448,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16" thickBot="1">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3528,7 +3500,7 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="3">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
@@ -3791,7 +3763,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="16" thickBot="1">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3807,7 +3779,7 @@
         <f t="shared" si="0"/>
         <v>152</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="7">
         <f t="shared" si="0"/>
         <v>153</v>
       </c>
@@ -3891,12 +3863,12 @@
         <f t="shared" si="1"/>
         <v>173</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="Z8" s="23">
         <f t="shared" si="1"/>
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="16" thickBot="1">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3932,7 +3904,7 @@
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="3">
         <f t="shared" si="0"/>
         <v>183</v>
       </c>
@@ -3972,7 +3944,7 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="T9" s="29">
+      <c r="T9" s="3">
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
@@ -3996,12 +3968,12 @@
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
-      <c r="Z9" s="24">
+      <c r="Z9" s="6">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="16" thickBot="1">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4029,7 +4001,7 @@
         <f t="shared" si="0"/>
         <v>205</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
         <v>206</v>
       </c>
@@ -4122,7 +4094,7 @@
         <f t="shared" si="0"/>
         <v>227</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>228</v>
       </c>
@@ -4421,7 +4393,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16" thickBot="1">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4497,7 +4469,7 @@
         <f t="shared" si="3"/>
         <v>317</v>
       </c>
-      <c r="T14" s="26">
+      <c r="T14" s="3">
         <f t="shared" si="3"/>
         <v>318</v>
       </c>
@@ -4526,7 +4498,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="16" thickBot="1">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4598,7 +4570,7 @@
         <f t="shared" si="3"/>
         <v>341</v>
       </c>
-      <c r="S15" s="29">
+      <c r="S15" s="3">
         <f t="shared" si="3"/>
         <v>342</v>
       </c>
@@ -4736,7 +4708,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="16" thickBot="1">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4841,7 +4813,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="16" thickBot="1">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4873,7 +4845,7 @@
         <f t="shared" si="2"/>
         <v>406</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="3">
         <f t="shared" si="2"/>
         <v>407</v>
       </c>
@@ -4913,7 +4885,7 @@
         <f t="shared" si="3"/>
         <v>416</v>
       </c>
-      <c r="S18" s="20">
+      <c r="S18" s="3">
         <f t="shared" si="3"/>
         <v>417</v>
       </c>
@@ -4946,11 +4918,11 @@
         <v>424</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="16" thickBot="1">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="5">
         <f t="shared" si="2"/>
         <v>425</v>
       </c>
@@ -4998,7 +4970,7 @@
         <f t="shared" si="3"/>
         <v>436</v>
       </c>
-      <c r="N19" s="27">
+      <c r="N19" s="7">
         <f t="shared" si="3"/>
         <v>437</v>
       </c>
@@ -5030,7 +5002,7 @@
         <f t="shared" si="3"/>
         <v>444</v>
       </c>
-      <c r="V19" s="28">
+      <c r="V19" s="3">
         <f t="shared" si="3"/>
         <v>445</v>
       </c>
@@ -5051,11 +5023,11 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="16" thickBot="1">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="20">
         <f t="shared" si="2"/>
         <v>450</v>
       </c>
@@ -5127,7 +5099,7 @@
         <f t="shared" si="3"/>
         <v>467</v>
       </c>
-      <c r="T20" s="30">
+      <c r="T20" s="3">
         <f t="shared" si="3"/>
         <v>468</v>
       </c>
@@ -5156,7 +5128,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="16" thickBot="1">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5232,7 +5204,7 @@
         <f t="shared" si="3"/>
         <v>492</v>
       </c>
-      <c r="T21" s="26">
+      <c r="T21" s="3">
         <f t="shared" si="3"/>
         <v>493</v>
       </c>
@@ -5261,7 +5233,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="16" thickBot="1">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5281,7 +5253,7 @@
         <f t="shared" si="2"/>
         <v>503</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="7">
         <f t="shared" si="2"/>
         <v>504</v>
       </c>
@@ -5543,7 +5515,7 @@
         <f t="shared" si="3"/>
         <v>566</v>
       </c>
-      <c r="S24" s="25">
+      <c r="S24" s="3">
         <f t="shared" si="3"/>
         <v>567</v>
       </c>
@@ -5713,7 +5685,7 @@
         <f t="shared" si="2"/>
         <v>606</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="4">
         <f t="shared" si="2"/>
         <v>607</v>
       </c>
@@ -5721,7 +5693,7 @@
         <f t="shared" si="2"/>
         <v>608</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="29">
         <f t="shared" si="2"/>
         <v>609</v>
       </c>
@@ -5745,7 +5717,7 @@
         <f t="shared" si="3"/>
         <v>614</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26" s="28">
         <f t="shared" si="3"/>
         <v>615</v>
       </c>

</xml_diff>

<commit_message>
Players are now passed into the board Players are now displayed on the board
</commit_message>
<xml_diff>
--- a/Finalized Board Layout.xlsx
+++ b/Finalized Board Layout.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17600" windowHeight="17760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z26" sqref="B2:Z26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3046,7 +3046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Detective notes now open when the button is pressed Added comments to a couple of different functions Slightly moved the room names on the board, added a spot for the Clost to have a name
</commit_message>
<xml_diff>
--- a/Finalized Board Layout.xlsx
+++ b/Finalized Board Layout.xlsx
@@ -825,7 +825,7 @@
   <dimension ref="A1:AG35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1644,23 +1644,23 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>4</v>
@@ -1727,7 +1727,7 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">

</xml_diff>